<commit_message>
remade schematic pdf and gerber files
</commit_message>
<xml_diff>
--- a/altium/ETL_RB/BOM/ETL_RB.xlsx
+++ b/altium/ETL_RB/BOM/ETL_RB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nemoz\Documents\readout-board-pcb\altium\ETL_RB\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{067326DD-6F02-4058-BDFA-5E6F4ED6FB30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B83C5E9-8D78-4E0E-A5D0-E54F3B43D281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="19200" windowHeight="10010" xr2:uid="{ACD2B078-0901-4531-9D25-645435820C86}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="19200" windowHeight="10010" xr2:uid="{3538EC13-96FA-4095-9CEE-522B485020D9}"/>
   </bookViews>
   <sheets>
     <sheet name="ETL_RB" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="112">
   <si>
     <t>Comment</t>
   </si>
@@ -281,7 +281,7 @@
     <t>120Kohm</t>
   </si>
   <si>
-    <t>R18, R21, R23, R25, R27, R28</t>
+    <t>R18, R21, R23, R25, R27</t>
   </si>
   <si>
     <t>RR0510P-102-D</t>
@@ -290,10 +290,19 @@
     <t>R19</t>
   </si>
   <si>
-    <t>50Mohm</t>
+    <t>3.9k</t>
+  </si>
+  <si>
+    <t>R28</t>
+  </si>
+  <si>
+    <t>HVC1206T5005JET</t>
   </si>
   <si>
     <t>R30, R31, R33, R34, R36, R37</t>
+  </si>
+  <si>
+    <t>resc3216n</t>
   </si>
   <si>
     <t>1.2Kohm</t>
@@ -741,8 +750,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56DDE4E1-F050-4200-831C-D82895C61C7C}">
-  <dimension ref="A1:F37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BA13ECD-C761-49A6-8FE6-A3DB8EA2F8F5}">
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1248,7 +1257,7 @@
         <v>61</v>
       </c>
       <c r="F25" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
@@ -1288,7 +1297,7 @@
         <v>61</v>
       </c>
       <c r="F27" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
@@ -1302,24 +1311,24 @@
         <v>86</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="F28" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>60</v>
@@ -1333,13 +1342,13 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>60</v>
@@ -1348,18 +1357,18 @@
         <v>61</v>
       </c>
       <c r="F30" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>60</v>
@@ -1373,13 +1382,13 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>60</v>
@@ -1393,22 +1402,22 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>61</v>
       </c>
       <c r="F33" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
@@ -1422,7 +1431,7 @@
         <v>99</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>61</v>
@@ -1433,16 +1442,16 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>61</v>
@@ -1453,19 +1462,19 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>103</v>
+        <v>58</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>104</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>105</v>
+        <v>61</v>
       </c>
       <c r="F36" s="1">
         <v>1</v>
@@ -1473,21 +1482,41 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>107</v>
       </c>
       <c r="D37" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="F37" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F38" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
regenerated pdf and gerber files
</commit_message>
<xml_diff>
--- a/altium/ETL_RB/BOM/ETL_RB.xlsx
+++ b/altium/ETL_RB/BOM/ETL_RB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nemoz\Documents\readout-board-pcb\altium\ETL_RB\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B83C5E9-8D78-4E0E-A5D0-E54F3B43D281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{22657235-2DE3-4F40-94A1-8B9189F0972E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="19200" windowHeight="10010" xr2:uid="{3538EC13-96FA-4095-9CEE-522B485020D9}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="19200" windowHeight="10010" xr2:uid="{3E0FC5B0-20BA-4592-BFC5-BFBA4BF70ADB}"/>
   </bookViews>
   <sheets>
     <sheet name="ETL_RB" sheetId="1" r:id="rId1"/>
@@ -750,7 +750,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BA13ECD-C761-49A6-8FE6-A3DB8EA2F8F5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52817B42-EDB7-4FCC-8DC7-ED5B8F514A4A}">
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>